<commit_message>
EA Peer Review update
Updates to rows for the following V-numbers:
V-81853
V-81855
V-81857
V-81879
V-81881
V-81897
V-81899
V-81911
V-81913
V-81915
V-81917
</commit_message>
<xml_diff>
--- a/cms-ars-3.1-moderate-mongodb-enterprise-advanced-3-stig-overlay.xlsx
+++ b/cms-ars-3.1-moderate-mongodb-enterprise-advanced-3-stig-overlay.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dhaynes/Documents/inspec/cms/cms-ars-3.1-moderate-mongodb-enterprise-advanced-3-stig-overlay/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\earonne\Desktop\Greg\Overlay_Worksheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{164C3207-16AB-FF46-9DBC-329C7D93F988}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{0293C25A-EF1A-46BD-B88D-976D60A8DFBD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cms-ars-3.1-moderate-mongodb-en" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'cms-ars-3.1-moderate-mongodb-en'!$A$1:$H$45</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="316" uniqueCount="268">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="321" uniqueCount="272">
   <si>
     <t>Vuln ID</t>
   </si>
@@ -358,14 +361,6 @@
     <t>Develop, document, and implement procedures to restrict and track use of the DBMS software installation account.</t>
   </si>
   <si>
-    <t xml:space="preserve">CCI-001499
-The organization limits privileges to change software resident within software libraries.
-NIST SP 800-53 :: CM-5 (6)
-NIST SP 800-53A :: CM-5 (6).1
-NIST SP 800-53 Revision 4 :: CM-5 (6)
-</t>
-  </si>
-  <si>
     <t>V-81855</t>
   </si>
   <si>
@@ -862,14 +857,6 @@
 Stop/start (restart) and mongod or mongos using the MongoDB configuration file.</t>
   </si>
   <si>
-    <t xml:space="preserve">CCI-001188
-The information system generates unique session identifiers for each session with organization-defined randomness requirements.
-NIST SP 800-53 :: SC-23 (4)
-NIST SP 800-53A :: SC-23 (4).1 (ii)
-NIST SP 800-53 Revision 4 :: SC-23 (3)
-</t>
-  </si>
-  <si>
     <t>V-81881</t>
   </si>
   <si>
@@ -1184,15 +1171,6 @@
 https://docs.mongodb.com/v3.4/reference/command/createRole/</t>
   </si>
   <si>
-    <t xml:space="preserve">CCI-002165
-The information system enforces organization-defined discretionary access control policies over defined subjects and objects.
-NIST SP 800-53 Revision 4 :: AC-3 (4)
-CCI-002235
-The information system prevents non-privileged users from executing privileged functions to include disabling, circumventing, or altering implemented security safeguards/countermeasures.
-NIST SP 800-53 Revision 4 :: AC-6 (10)
-</t>
-  </si>
-  <si>
     <t>V-81901</t>
   </si>
   <si>
@@ -1357,12 +1335,6 @@
 To revoke a user's role from a database use the db.revokeRolesFromUser() method.
 https://docs.mongodb.com/v3.4/reference/method/db.revokeRolesFromUser/
 To grant a role to a user use the db.grantRolesToUser() method. https://docs.mongodb.com/v3.4/reference/method/db.grantRolesToUser/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CCI-001813
-The information system enforces access restrictions.
-NIST SP 800-53 Revision 4 :: CM-5 (1)
-</t>
   </si>
   <si>
     <t>V-81913</t>
@@ -2602,12 +2574,151 @@
 If the MongoDB is not configured in accordance with security configuration settings, this is a finding.</t>
     </r>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <strike/>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">CCI-001499
+The organization limits privileges to change software resident within software libraries.
+NIST SP 800-53 :: CM-5 (6)
+NIST SP 800-53A :: CM-5 (6).1
+NIST SP 800-53 Revision 4 :: CM-5 (6)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">CM-5
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <strike/>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">CCI-001188
+The information system generates unique session identifiers for each session with organization-defined randomness requirements.
+NIST SP 800-53 :: SC-23 (4)
+NIST SP 800-53A :: SC-23 (4).1 (ii)
+NIST SP 800-53 Revision 4 :: SC-23 (3)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">SC-23
+</t>
+    </r>
+  </si>
+  <si>
+    <t>(not in ARS)
+Add to Overlay:
+desc, 'caveat', 'Not applicable for this CMS ARS 3.1 overlay, since the related security control is not applied to this system categorization in CMS ARS 3.1'</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>(not in ARS)
+Add to Overlay:
+desc, 'caveat', 'Not applicable for this CMS ARS 3.1 overlay, since the related security control is not mandatory in CMS ARS 3.1'</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">CCI-002165
+The information system enforces organization-defined discretionary access control policies over defined subjects and objects.
+NIST SP 800-53 Revision 4 :: AC-3 (4)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+CCI-002235
+The information system prevents non-privileged users from executing privileged functions to include disabling, circumventing, or altering implemented security safeguards/countermeasures.
+NIST SP 800-53 Revision 4 :: AC-6 (10)
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <strike/>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">CCI-001813
+The information system enforces access restrictions.
+NIST SP 800-53 Revision 4 :: CM-5 (1)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">CM-5
+</t>
+    </r>
+  </si>
+  <si>
+    <t>(not in ARS)
+Add to Overlay:
+desc, 'caveat', 'Not applicable for this CMS ARS 3.1 overlay, since the related security control is not included in CMS ARS 3.1'</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19">
+  <fonts count="22">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2747,6 +2858,31 @@
       <sz val="12"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="12"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <strike/>
+      <sz val="12"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="34">
@@ -2936,7 +3072,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <start/>
       <end/>
@@ -3051,6 +3187,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <start style="thin">
+        <color indexed="64"/>
+      </start>
+      <end style="thin">
+        <color indexed="64"/>
+      </end>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -3096,7 +3247,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -3104,13 +3255,22 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="6" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="6" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="7" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="10" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3470,1061 +3630,1117 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A45" sqref="A45"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="10.84765625" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="8.6640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.6484375" style="1" customWidth="1"/>
     <col min="2" max="2" width="10" style="1" customWidth="1"/>
-    <col min="3" max="3" width="28.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="27.1640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="20.6640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="20" style="1" customWidth="1"/>
-    <col min="7" max="7" width="21.1640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="20.1640625" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="1"/>
+    <col min="3" max="3" width="22.84765625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="48.1484375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="39.94921875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="45.34765625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="21.1484375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="20.1484375" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="10.84765625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1" ht="17">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:8" s="2" customFormat="1">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="3" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="390">
+      <c r="A2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="5"/>
+    </row>
+    <row r="3" spans="1:8" ht="265.2">
+      <c r="A3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="5"/>
+    </row>
+    <row r="4" spans="1:8" ht="409.5">
+      <c r="A4" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" s="5"/>
+    </row>
+    <row r="5" spans="1:8" ht="409.5">
+      <c r="A5" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" s="5"/>
+    </row>
+    <row r="6" spans="1:8" ht="409.5">
+      <c r="A6" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H6" s="5"/>
+    </row>
+    <row r="7" spans="1:8" ht="358.8">
+      <c r="A7" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>264</v>
+      </c>
+      <c r="H7" s="5"/>
+    </row>
+    <row r="8" spans="1:8" ht="327.60000000000002">
+      <c r="A8" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>264</v>
+      </c>
+      <c r="H8" s="5"/>
+    </row>
+    <row r="9" spans="1:8" ht="343.2">
+      <c r="A9" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>264</v>
+      </c>
+      <c r="H9" s="5"/>
+    </row>
+    <row r="10" spans="1:8" ht="249.6">
+      <c r="A10" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="H10" s="5"/>
+    </row>
+    <row r="11" spans="1:8" ht="409.5">
+      <c r="A11" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="H11" s="5"/>
+    </row>
+    <row r="12" spans="1:8" ht="390">
+      <c r="A12" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="H12" s="5"/>
+    </row>
+    <row r="13" spans="1:8" ht="265.2">
+      <c r="A13" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="D13" s="7" t="s">
         <v>248</v>
       </c>
+      <c r="E13" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="H13" s="5"/>
     </row>
-    <row r="2" spans="1:8" ht="409.6">
-      <c r="A2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="1" t="s">
+    <row r="14" spans="1:8" ht="409.5">
+      <c r="A14" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="C14" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="H14" s="5"/>
     </row>
-    <row r="3" spans="1:8" ht="409.6">
-      <c r="A3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="1" t="s">
+    <row r="15" spans="1:8" ht="409.5">
+      <c r="A15" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B15" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>17</v>
-      </c>
+      <c r="C15" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="H15" s="5"/>
     </row>
-    <row r="4" spans="1:8" ht="409.6">
-      <c r="A4" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="1" t="s">
+    <row r="16" spans="1:8" ht="409.5">
+      <c r="A16" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="H16" s="5"/>
+    </row>
+    <row r="17" spans="1:8" ht="409.5">
+      <c r="A17" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>249</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>250</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>21</v>
-      </c>
+      <c r="C17" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>252</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="H17" s="5"/>
     </row>
-    <row r="5" spans="1:8" ht="409.6">
-      <c r="A5" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" s="1" t="s">
+    <row r="18" spans="1:8" ht="409.5">
+      <c r="A18" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="H18" s="5"/>
+    </row>
+    <row r="19" spans="1:8" ht="409.5">
+      <c r="A19" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B19" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>27</v>
-      </c>
+      <c r="C19" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="H19" s="5"/>
     </row>
-    <row r="6" spans="1:8" ht="409.6">
-      <c r="A6" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B6" s="1" t="s">
+    <row r="20" spans="1:8" ht="265.2">
+      <c r="A20" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="B20" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>33</v>
-      </c>
+      <c r="C20" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>265</v>
+      </c>
+      <c r="H20" s="5"/>
     </row>
-    <row r="7" spans="1:8" ht="409.6">
-      <c r="A7" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" s="1" t="s">
+    <row r="21" spans="1:8" ht="409.5">
+      <c r="A21" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>267</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="H21" s="8" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="296.39999999999998">
+      <c r="A22" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B22" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>39</v>
-      </c>
+      <c r="C22" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="H22" s="5"/>
     </row>
-    <row r="8" spans="1:8" ht="409.6">
-      <c r="A8" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B8" s="1" t="s">
+    <row r="23" spans="1:8" ht="249.6">
+      <c r="A23" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="B23" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>39</v>
-      </c>
+      <c r="C23" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="H23" s="5"/>
     </row>
-    <row r="9" spans="1:8" ht="409.6">
-      <c r="A9" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B9" s="1" t="s">
+    <row r="24" spans="1:8" ht="202.8">
+      <c r="A24" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B24" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>39</v>
-      </c>
+      <c r="C24" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="H24" s="5"/>
     </row>
-    <row r="10" spans="1:8" ht="409.6">
-      <c r="A10" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B10" s="1" t="s">
+    <row r="25" spans="1:8" ht="409.5">
+      <c r="A25" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="B25" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>55</v>
-      </c>
+      <c r="C25" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="H25" s="5"/>
     </row>
-    <row r="11" spans="1:8" ht="409.6">
-      <c r="A11" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B11" s="1" t="s">
+    <row r="26" spans="1:8" ht="409.5">
+      <c r="A26" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="B26" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>61</v>
-      </c>
+      <c r="C26" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="H26" s="5"/>
     </row>
-    <row r="12" spans="1:8" ht="409.6">
-      <c r="A12" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B12" s="1" t="s">
+    <row r="27" spans="1:8" ht="409.5">
+      <c r="A27" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="B27" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>67</v>
-      </c>
+      <c r="C27" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="H27" s="5"/>
     </row>
-    <row r="13" spans="1:8" ht="409.6">
-      <c r="A13" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B13" s="1" t="s">
+    <row r="28" spans="1:8" ht="409.5">
+      <c r="A28" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="B28" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>251</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>252</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>71</v>
-      </c>
+      <c r="C28" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="H28" s="5"/>
     </row>
-    <row r="14" spans="1:8" ht="409.6">
-      <c r="A14" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="B14" s="1" t="s">
+    <row r="29" spans="1:8" ht="409.5">
+      <c r="A29" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>267</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="H29" s="8" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="409.5">
+      <c r="A30" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="B30" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D14" s="4" t="s">
+      <c r="C30" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="G30" s="7" t="s">
+        <v>269</v>
+      </c>
+      <c r="H30" s="5"/>
+    </row>
+    <row r="31" spans="1:8" ht="280.8">
+      <c r="A31" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="H31" s="5"/>
+    </row>
+    <row r="32" spans="1:8" ht="280.8">
+      <c r="A32" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="G32" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="H32" s="5"/>
+    </row>
+    <row r="33" spans="1:8" ht="409.5">
+      <c r="A33" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="H33" s="5"/>
+    </row>
+    <row r="34" spans="1:8" ht="280.8">
+      <c r="A34" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C34" s="7" t="s">
         <v>253</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>76</v>
-      </c>
+      <c r="D34" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="F34" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="G34" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="H34" s="5"/>
     </row>
-    <row r="15" spans="1:8" ht="409.6">
-      <c r="A15" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="B15" s="1" t="s">
+    <row r="35" spans="1:8" ht="409.5">
+      <c r="A35" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="B35" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>254</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>81</v>
-      </c>
+      <c r="C35" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="H35" s="5"/>
     </row>
-    <row r="16" spans="1:8" ht="409.6">
-      <c r="A16" s="5" t="s">
+    <row r="36" spans="1:8" ht="409.5">
+      <c r="A36" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="G36" s="8" t="s">
+        <v>270</v>
+      </c>
+      <c r="H36" s="5"/>
+    </row>
+    <row r="37" spans="1:8" ht="409.5">
+      <c r="A37" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>267</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="G37" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="H37" s="8" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="327.60000000000002">
+      <c r="A38" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>267</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="G38" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="H38" s="8" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="218.4">
+      <c r="A39" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>267</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>257</v>
+      </c>
+      <c r="E39" s="7" t="s">
+        <v>258</v>
+      </c>
+      <c r="F39" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="G39" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="H39" s="8" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="374.4">
+      <c r="A40" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="G40" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="H40" s="5"/>
+    </row>
+    <row r="41" spans="1:8" ht="296.39999999999998">
+      <c r="A41" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="G41" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="H41" s="5"/>
+    </row>
+    <row r="42" spans="1:8" ht="296.39999999999998">
+      <c r="A42" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="F42" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="G42" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="H42" s="5"/>
+    </row>
+    <row r="43" spans="1:8" ht="374.4">
+      <c r="A43" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="E43" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="F43" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="G43" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="H43" s="5"/>
+    </row>
+    <row r="44" spans="1:8" ht="409.5">
+      <c r="A44" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="B44" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>255</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>87</v>
-      </c>
+      <c r="C44" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="F44" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="G44" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="H44" s="5"/>
     </row>
-    <row r="17" spans="1:7" ht="409.6">
-      <c r="A17" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="B17" s="1" t="s">
+    <row r="45" spans="1:8" ht="187.2">
+      <c r="A45" s="6" t="s">
+        <v>241</v>
+      </c>
+      <c r="B45" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>256</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="409.6">
-      <c r="A18" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="409.6">
-      <c r="A19" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="388">
-      <c r="A20" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="409.6">
-      <c r="A21" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="409.6">
-      <c r="A22" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="409.6">
-      <c r="A23" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="388">
-      <c r="A24" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="409.6">
-      <c r="A25" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="409.6">
-      <c r="A26" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="409.6">
-      <c r="A27" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="409.6">
-      <c r="A28" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="409.6">
-      <c r="A29" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="409.6">
-      <c r="A30" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="409.6">
-      <c r="A31" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="409.6">
-      <c r="A32" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="409.6">
-      <c r="A33" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="409.6">
-      <c r="A34" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>257</v>
-      </c>
-      <c r="D34" s="4" t="s">
-        <v>258</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="F34" s="4" t="s">
-        <v>259</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="409.6">
-      <c r="A35" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="G35" s="1" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="409.6">
-      <c r="A36" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" ht="409.6">
-      <c r="A37" s="3" t="s">
-        <v>202</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="G37" s="1" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="409.6">
-      <c r="A38" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="G38" s="1" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" ht="409.6">
-      <c r="A39" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>260</v>
-      </c>
-      <c r="D39" s="4" t="s">
+      <c r="C45" s="7" t="s">
         <v>261</v>
       </c>
-      <c r="E39" s="4" t="s">
+      <c r="D45" s="7" t="s">
         <v>262</v>
       </c>
-      <c r="F39" s="4" t="s">
+      <c r="E45" s="7" t="s">
         <v>263</v>
       </c>
-      <c r="G39" s="1" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" ht="409.6">
-      <c r="A40" s="3" t="s">
-        <v>216</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="G40" s="1" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" ht="409.6">
-      <c r="A41" s="3" t="s">
-        <v>222</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="G41" s="1" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="409.6">
-      <c r="A42" s="5" t="s">
-        <v>228</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="F42" s="4" t="s">
-        <v>264</v>
-      </c>
-      <c r="G42" s="1" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" ht="409.6">
-      <c r="A43" s="3" t="s">
-        <v>233</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="G43" s="1" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" ht="409.6">
-      <c r="A44" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="E44" s="1" t="s">
+      <c r="F45" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="F44" s="1" t="s">
+      <c r="G45" s="5" t="s">
         <v>243</v>
       </c>
-      <c r="G44" s="1" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" ht="356">
-      <c r="A45" s="5" t="s">
-        <v>245</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>265</v>
-      </c>
-      <c r="D45" s="4" t="s">
-        <v>266</v>
-      </c>
-      <c r="E45" s="4" t="s">
-        <v>267</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="G45" s="1" t="s">
-        <v>247</v>
-      </c>
+      <c r="H45" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
updating spreadsheet and overlay based on EA feedback
</commit_message>
<xml_diff>
--- a/cms-ars-3.1-moderate-mongodb-enterprise-advanced-3-stig-overlay.xlsx
+++ b/cms-ars-3.1-moderate-mongodb-enterprise-advanced-3-stig-overlay.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\earonne\Desktop\Greg\Overlay_Worksheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dhaynes/Documents/inspec/cms/cms-ars-3.1-moderate-mongodb-enterprise-advanced-3-stig-overlay/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{0293C25A-EF1A-46BD-B88D-976D60A8DFBD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{54EAB094-5560-364B-9B63-70FBC5B2FC38}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="67200" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cms-ars-3.1-moderate-mongodb-en" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="321" uniqueCount="272">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="321" uniqueCount="274">
   <si>
     <t>Vuln ID</t>
   </si>
@@ -2575,6 +2575,54 @@
     </r>
   </si>
   <si>
+    <t>(not in ARS)
+Add to Overlay:
+desc, 'caveat', 'Not applicable for this CMS ARS 3.1 overlay, since the related security control is not applied to this system categorization in CMS ARS 3.1'</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>(not in ARS)
+Add to Overlay:
+desc, 'caveat', 'Not applicable for this CMS ARS 3.1 overlay, since the related security control is not mandatory in CMS ARS 3.1'</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">CCI-002165
+The information system enforces organization-defined discretionary access control policies over defined subjects and objects.
+NIST SP 800-53 Revision 4 :: AC-3 (4)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+CCI-002235
+The information system prevents non-privileged users from executing privileged functions to include disabling, circumventing, or altering implemented security safeguards/countermeasures.
+NIST SP 800-53 Revision 4 :: AC-6 (10)
+</t>
+    </r>
+  </si>
+  <si>
+    <t>(not in ARS)
+Add to Overlay:
+desc, 'caveat', 'Not applicable for this CMS ARS 3.1 overlay, since the related security control is not included in CMS ARS 3.1'</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -2601,8 +2649,68 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">CM-5
+      <t xml:space="preserve">
+CCI-000338
+The organization defines physical access restrictions associated with changes to the information system.
+NIST SP 800-53::CM-5
+NIST SP 800-53 Revision 4::CM 5
 </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <strike/>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">CCI-001499
+The organization limits privileges to change software resident within software libraries.
+NIST SP 800-53 :: CM-5 (6)
+NIST SP 800-53A :: CM-5 (6).1
+NIST SP 800-53 Revision 4 :: CM-5 (6)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+CCI-000338
+The organization defines physical access restrictions associated with changes to the information system.
+NIST SP 800-53::CM-5
+NIST SP 800-53 Revision 4::CM 5</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">CCI-001499
+The organization limits privileges to change software resident within software libraries.
+NIST SP 800-53 :: CM-5 (6)
+NIST SP 800-53A :: CM-5 (6).1
+NIST SP 800-53 Revision 4 :: CM-5 (6)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>CCI-000338
+The organization defines physical access restrictions associated with changes to the information system.
+NIST SP 800-53::CM-5
+NIST SP 800-53 Revision 4::CM 5</t>
     </r>
   </si>
   <si>
@@ -2632,50 +2740,12 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">SC-23
-</t>
-    </r>
-  </si>
-  <si>
-    <t>(not in ARS)
-Add to Overlay:
-desc, 'caveat', 'Not applicable for this CMS ARS 3.1 overlay, since the related security control is not applied to this system categorization in CMS ARS 3.1'</t>
-  </si>
-  <si>
-    <t>none</t>
-  </si>
-  <si>
-    <t>(not in ARS)
-Add to Overlay:
-desc, 'caveat', 'Not applicable for this CMS ARS 3.1 overlay, since the related security control is not mandatory in CMS ARS 3.1'</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="12"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">CCI-002165
-The information system enforces organization-defined discretionary access control policies over defined subjects and objects.
-NIST SP 800-53 Revision 4 :: AC-3 (4)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t xml:space="preserve">
-CCI-002235
-The information system prevents non-privileged users from executing privileged functions to include disabling, circumventing, or altering implemented security safeguards/countermeasures.
-NIST SP 800-53 Revision 4 :: AC-6 (10)
+CCI-001184
+The information system protects the authenticity of communications sessions.
+NIST SP 800-53::SC-23
+NIST SP 800-53A::SC-23
+NIST SP 800-53 Revision 4::SC-23
 </t>
     </r>
   </si>
@@ -2704,21 +2774,19 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">CM-5
-</t>
-    </r>
-  </si>
-  <si>
-    <t>(not in ARS)
-Add to Overlay:
-desc, 'caveat', 'Not applicable for this CMS ARS 3.1 overlay, since the related security control is not included in CMS ARS 3.1'</t>
+      <t xml:space="preserve">
+CCI-000338
+The organization defines physical access restrictions associated with changes to the information system.
+NIST SP 800-53::CM-5
+NIST SP 800-53 Revision 4::CM 5</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2883,6 +2951,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri (Body)"/>
     </font>
   </fonts>
   <fills count="34">
@@ -3247,7 +3321,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -3271,6 +3345,9 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3630,27 +3707,27 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozenSplit"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B38" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.84765625" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="8.6484375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="10" style="1" customWidth="1"/>
-    <col min="3" max="3" width="22.84765625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="48.1484375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="39.94921875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="45.34765625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="21.1484375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="20.1484375" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="10.84765625" style="1"/>
+    <col min="3" max="3" width="22.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="48.1640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="40" style="1" customWidth="1"/>
+    <col min="6" max="6" width="45.33203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="21.1640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="20.1640625" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1">
+    <row r="1" spans="1:8" s="2" customFormat="1" ht="17">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -3676,7 +3753,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="390">
+    <row r="2" spans="1:8" ht="409.6">
       <c r="A2" s="4" t="s">
         <v>7</v>
       </c>
@@ -3700,7 +3777,7 @@
       </c>
       <c r="H2" s="5"/>
     </row>
-    <row r="3" spans="1:8" ht="265.2">
+    <row r="3" spans="1:8" ht="306">
       <c r="A3" s="4" t="s">
         <v>13</v>
       </c>
@@ -3724,7 +3801,7 @@
       </c>
       <c r="H3" s="5"/>
     </row>
-    <row r="4" spans="1:8" ht="409.5">
+    <row r="4" spans="1:8" ht="409.6">
       <c r="A4" s="6" t="s">
         <v>18</v>
       </c>
@@ -3748,7 +3825,7 @@
       </c>
       <c r="H4" s="5"/>
     </row>
-    <row r="5" spans="1:8" ht="409.5">
+    <row r="5" spans="1:8" ht="409.6">
       <c r="A5" s="4" t="s">
         <v>22</v>
       </c>
@@ -3772,7 +3849,7 @@
       </c>
       <c r="H5" s="5"/>
     </row>
-    <row r="6" spans="1:8" ht="409.5">
+    <row r="6" spans="1:8" ht="409.6">
       <c r="A6" s="4" t="s">
         <v>28</v>
       </c>
@@ -3796,7 +3873,7 @@
       </c>
       <c r="H6" s="5"/>
     </row>
-    <row r="7" spans="1:8" ht="358.8">
+    <row r="7" spans="1:8" ht="404">
       <c r="A7" s="6" t="s">
         <v>34</v>
       </c>
@@ -3816,11 +3893,11 @@
         <v>38</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>264</v>
+        <v>269</v>
       </c>
       <c r="H7" s="5"/>
     </row>
-    <row r="8" spans="1:8" ht="327.60000000000002">
+    <row r="8" spans="1:8" ht="372">
       <c r="A8" s="6" t="s">
         <v>39</v>
       </c>
@@ -3840,11 +3917,11 @@
         <v>43</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>264</v>
+        <v>270</v>
       </c>
       <c r="H8" s="5"/>
     </row>
-    <row r="9" spans="1:8" ht="343.2">
+    <row r="9" spans="1:8" ht="372">
       <c r="A9" s="6" t="s">
         <v>44</v>
       </c>
@@ -3863,12 +3940,12 @@
       <c r="F9" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="G9" s="8" t="s">
-        <v>264</v>
+      <c r="G9" s="9" t="s">
+        <v>271</v>
       </c>
       <c r="H9" s="5"/>
     </row>
-    <row r="10" spans="1:8" ht="249.6">
+    <row r="10" spans="1:8" ht="289">
       <c r="A10" s="4" t="s">
         <v>49</v>
       </c>
@@ -3892,7 +3969,7 @@
       </c>
       <c r="H10" s="5"/>
     </row>
-    <row r="11" spans="1:8" ht="409.5">
+    <row r="11" spans="1:8" ht="409.6">
       <c r="A11" s="4" t="s">
         <v>55</v>
       </c>
@@ -3916,7 +3993,7 @@
       </c>
       <c r="H11" s="5"/>
     </row>
-    <row r="12" spans="1:8" ht="390">
+    <row r="12" spans="1:8" ht="409.6">
       <c r="A12" s="4" t="s">
         <v>61</v>
       </c>
@@ -3940,7 +4017,7 @@
       </c>
       <c r="H12" s="5"/>
     </row>
-    <row r="13" spans="1:8" ht="265.2">
+    <row r="13" spans="1:8" ht="323">
       <c r="A13" s="6" t="s">
         <v>67</v>
       </c>
@@ -3964,7 +4041,7 @@
       </c>
       <c r="H13" s="5"/>
     </row>
-    <row r="14" spans="1:8" ht="409.5">
+    <row r="14" spans="1:8" ht="409.6">
       <c r="A14" s="6" t="s">
         <v>71</v>
       </c>
@@ -3988,7 +4065,7 @@
       </c>
       <c r="H14" s="5"/>
     </row>
-    <row r="15" spans="1:8" ht="409.5">
+    <row r="15" spans="1:8" ht="409.6">
       <c r="A15" s="6" t="s">
         <v>76</v>
       </c>
@@ -4012,7 +4089,7 @@
       </c>
       <c r="H15" s="5"/>
     </row>
-    <row r="16" spans="1:8" ht="409.5">
+    <row r="16" spans="1:8" ht="409.6">
       <c r="A16" s="6" t="s">
         <v>81</v>
       </c>
@@ -4036,7 +4113,7 @@
       </c>
       <c r="H16" s="5"/>
     </row>
-    <row r="17" spans="1:8" ht="409.5">
+    <row r="17" spans="1:8" ht="409.6">
       <c r="A17" s="6" t="s">
         <v>87</v>
       </c>
@@ -4060,7 +4137,7 @@
       </c>
       <c r="H17" s="5"/>
     </row>
-    <row r="18" spans="1:8" ht="409.5">
+    <row r="18" spans="1:8" ht="409.6">
       <c r="A18" s="4" t="s">
         <v>92</v>
       </c>
@@ -4084,7 +4161,7 @@
       </c>
       <c r="H18" s="5"/>
     </row>
-    <row r="19" spans="1:8" ht="409.5">
+    <row r="19" spans="1:8" ht="409.6">
       <c r="A19" s="4" t="s">
         <v>98</v>
       </c>
@@ -4108,7 +4185,7 @@
       </c>
       <c r="H19" s="5"/>
     </row>
-    <row r="20" spans="1:8" ht="265.2">
+    <row r="20" spans="1:8" ht="409.6">
       <c r="A20" s="6" t="s">
         <v>104</v>
       </c>
@@ -4128,16 +4205,16 @@
         <v>108</v>
       </c>
       <c r="G20" s="8" t="s">
-        <v>265</v>
+        <v>272</v>
       </c>
       <c r="H20" s="5"/>
     </row>
-    <row r="21" spans="1:8" ht="409.5">
+    <row r="21" spans="1:8" ht="409.6">
       <c r="A21" s="6" t="s">
         <v>109</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>110</v>
@@ -4155,10 +4232,10 @@
         <v>114</v>
       </c>
       <c r="H21" s="8" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="296.39999999999998">
+    <row r="22" spans="1:8" ht="323">
       <c r="A22" s="4" t="s">
         <v>115</v>
       </c>
@@ -4182,7 +4259,7 @@
       </c>
       <c r="H22" s="5"/>
     </row>
-    <row r="23" spans="1:8" ht="249.6">
+    <row r="23" spans="1:8" ht="272">
       <c r="A23" s="4" t="s">
         <v>121</v>
       </c>
@@ -4206,7 +4283,7 @@
       </c>
       <c r="H23" s="5"/>
     </row>
-    <row r="24" spans="1:8" ht="202.8">
+    <row r="24" spans="1:8" ht="238">
       <c r="A24" s="4" t="s">
         <v>127</v>
       </c>
@@ -4230,7 +4307,7 @@
       </c>
       <c r="H24" s="5"/>
     </row>
-    <row r="25" spans="1:8" ht="409.5">
+    <row r="25" spans="1:8" ht="409.6">
       <c r="A25" s="4" t="s">
         <v>132</v>
       </c>
@@ -4254,7 +4331,7 @@
       </c>
       <c r="H25" s="5"/>
     </row>
-    <row r="26" spans="1:8" ht="409.5">
+    <row r="26" spans="1:8" ht="409.6">
       <c r="A26" s="4" t="s">
         <v>138</v>
       </c>
@@ -4278,7 +4355,7 @@
       </c>
       <c r="H26" s="5"/>
     </row>
-    <row r="27" spans="1:8" ht="409.5">
+    <row r="27" spans="1:8" ht="409.6">
       <c r="A27" s="4" t="s">
         <v>143</v>
       </c>
@@ -4302,7 +4379,7 @@
       </c>
       <c r="H27" s="5"/>
     </row>
-    <row r="28" spans="1:8" ht="409.5">
+    <row r="28" spans="1:8" ht="409.6">
       <c r="A28" s="4" t="s">
         <v>149</v>
       </c>
@@ -4326,12 +4403,12 @@
       </c>
       <c r="H28" s="5"/>
     </row>
-    <row r="29" spans="1:8" ht="409.5">
+    <row r="29" spans="1:8" ht="409.6">
       <c r="A29" s="6" t="s">
         <v>155</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>156</v>
@@ -4349,10 +4426,10 @@
         <v>160</v>
       </c>
       <c r="H29" s="8" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="409.5">
+    <row r="30" spans="1:8" ht="409.6">
       <c r="A30" s="6" t="s">
         <v>161</v>
       </c>
@@ -4372,11 +4449,11 @@
         <v>165</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="H30" s="5"/>
     </row>
-    <row r="31" spans="1:8" ht="280.8">
+    <row r="31" spans="1:8" ht="323">
       <c r="A31" s="4" t="s">
         <v>166</v>
       </c>
@@ -4400,7 +4477,7 @@
       </c>
       <c r="H31" s="5"/>
     </row>
-    <row r="32" spans="1:8" ht="280.8">
+    <row r="32" spans="1:8" ht="323">
       <c r="A32" s="4" t="s">
         <v>172</v>
       </c>
@@ -4424,7 +4501,7 @@
       </c>
       <c r="H32" s="5"/>
     </row>
-    <row r="33" spans="1:8" ht="409.5">
+    <row r="33" spans="1:8" ht="409.6">
       <c r="A33" s="4" t="s">
         <v>178</v>
       </c>
@@ -4448,7 +4525,7 @@
       </c>
       <c r="H33" s="5"/>
     </row>
-    <row r="34" spans="1:8" ht="280.8">
+    <row r="34" spans="1:8" ht="323">
       <c r="A34" s="6" t="s">
         <v>184</v>
       </c>
@@ -4472,7 +4549,7 @@
       </c>
       <c r="H34" s="5"/>
     </row>
-    <row r="35" spans="1:8" ht="409.5">
+    <row r="35" spans="1:8" ht="409.6">
       <c r="A35" s="4" t="s">
         <v>187</v>
       </c>
@@ -4496,7 +4573,7 @@
       </c>
       <c r="H35" s="5"/>
     </row>
-    <row r="36" spans="1:8" ht="409.5">
+    <row r="36" spans="1:8" ht="409.6">
       <c r="A36" s="6" t="s">
         <v>193</v>
       </c>
@@ -4516,16 +4593,16 @@
         <v>197</v>
       </c>
       <c r="G36" s="8" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="H36" s="5"/>
     </row>
-    <row r="37" spans="1:8" ht="409.5">
+    <row r="37" spans="1:8" ht="409.6">
       <c r="A37" s="6" t="s">
         <v>198</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>199</v>
@@ -4543,15 +4620,15 @@
         <v>203</v>
       </c>
       <c r="H37" s="8" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="327.60000000000002">
+    <row r="38" spans="1:8" ht="372">
       <c r="A38" s="6" t="s">
         <v>204</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>205</v>
@@ -4569,15 +4646,15 @@
         <v>209</v>
       </c>
       <c r="H38" s="8" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="218.4">
+    <row r="39" spans="1:8" ht="272">
       <c r="A39" s="6" t="s">
         <v>210</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C39" s="7" t="s">
         <v>256</v>
@@ -4595,10 +4672,10 @@
         <v>211</v>
       </c>
       <c r="H39" s="8" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="374.4">
+    <row r="40" spans="1:8" ht="404">
       <c r="A40" s="4" t="s">
         <v>212</v>
       </c>
@@ -4622,7 +4699,7 @@
       </c>
       <c r="H40" s="5"/>
     </row>
-    <row r="41" spans="1:8" ht="296.39999999999998">
+    <row r="41" spans="1:8" ht="323">
       <c r="A41" s="4" t="s">
         <v>218</v>
       </c>
@@ -4646,7 +4723,7 @@
       </c>
       <c r="H41" s="5"/>
     </row>
-    <row r="42" spans="1:8" ht="296.39999999999998">
+    <row r="42" spans="1:8" ht="340">
       <c r="A42" s="6" t="s">
         <v>224</v>
       </c>
@@ -4670,7 +4747,7 @@
       </c>
       <c r="H42" s="5"/>
     </row>
-    <row r="43" spans="1:8" ht="374.4">
+    <row r="43" spans="1:8" ht="404">
       <c r="A43" s="4" t="s">
         <v>229</v>
       </c>
@@ -4694,7 +4771,7 @@
       </c>
       <c r="H43" s="5"/>
     </row>
-    <row r="44" spans="1:8" ht="409.5">
+    <row r="44" spans="1:8" ht="409.6">
       <c r="A44" s="4" t="s">
         <v>235</v>
       </c>
@@ -4718,7 +4795,7 @@
       </c>
       <c r="H44" s="5"/>
     </row>
-    <row r="45" spans="1:8" ht="187.2">
+    <row r="45" spans="1:8" ht="204">
       <c r="A45" s="6" t="s">
         <v>241</v>
       </c>

</xml_diff>